<commit_message>
Added guild and species of concern columns
</commit_message>
<xml_diff>
--- a/species_traits.xlsx
+++ b/species_traits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelly\Documents\Belize-MP-Bruno-Boos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4788EDD9-BCA6-774D-B8C1-40C46D2104CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BA0721-9B22-4DB8-ADAA-7BB222FE480C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1000" windowWidth="28420" windowHeight="16100" xr2:uid="{FB4CAFAA-C94C-0A41-A350-C1EADAEBA5A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{FB4CAFAA-C94C-0A41-A350-C1EADAEBA5A6}"/>
   </bookViews>
   <sheets>
     <sheet name="species_traits" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="111">
   <si>
     <t>Common Name</t>
   </si>
@@ -342,6 +342,33 @@
   </si>
   <si>
     <t>Ocellated turkey</t>
+  </si>
+  <si>
+    <t>Guild</t>
+  </si>
+  <si>
+    <t>Species_of_concern</t>
+  </si>
+  <si>
+    <t>Ungulate</t>
+  </si>
+  <si>
+    <t>Carnivore</t>
+  </si>
+  <si>
+    <t>Insectivore</t>
+  </si>
+  <si>
+    <t>Generalist</t>
+  </si>
+  <si>
+    <t>Frugivore</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -391,11 +418,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,13 +736,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93F3431-E395-8C41-A97B-835F042CB4DC}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
@@ -724,7 +750,7 @@
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,8 +772,14 @@
       <c r="G1" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -769,8 +801,14 @@
       <c r="G2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -792,8 +830,14 @@
       <c r="G3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -815,8 +859,14 @@
       <c r="G4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -838,8 +888,14 @@
       <c r="G5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -861,8 +917,14 @@
       <c r="G6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -884,8 +946,14 @@
       <c r="G7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -907,8 +975,14 @@
       <c r="G8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -930,8 +1004,14 @@
       <c r="G9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -953,8 +1033,14 @@
       <c r="G10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -976,8 +1062,14 @@
       <c r="G11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -999,8 +1091,14 @@
       <c r="G12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1022,8 +1120,14 @@
       <c r="G13" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -1045,8 +1149,14 @@
       <c r="G14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1068,8 +1178,14 @@
       <c r="G15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1091,8 +1207,14 @@
       <c r="G16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -1114,31 +1236,43 @@
       <c r="G17" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="H17" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1160,8 +1294,14 @@
       <c r="G19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1183,8 +1323,14 @@
       <c r="G20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1206,8 +1352,14 @@
       <c r="G21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1229,8 +1381,14 @@
       <c r="G22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -1252,8 +1410,14 @@
       <c r="G23" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -1275,8 +1439,14 @@
       <c r="G24" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1298,8 +1468,14 @@
       <c r="G25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1321,12 +1497,18 @@
       <c r="G26" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>36</v>
       </c>
       <c r="C27" t="s">
@@ -1344,8 +1526,14 @@
       <c r="G27" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1367,11 +1555,17 @@
       <c r="G28" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
   </sheetData>
@@ -1379,5 +1573,6 @@
     <sortCondition ref="F2:F28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>